<commit_message>
update other compensation info
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\q-definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7B8FFE58-C504-4507-8DCC-B08B846CCC89}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE46E38-B6AB-42B8-85A3-98D21CBEF030}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32772" yWindow="32772" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="32772" yWindow="32772" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="2" r:id="rId1"/>
@@ -18,24 +18,16 @@
     <sheet name="English police forces" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Dictionary'!$A$2:$L$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data Dictionary'!$A$2:$L$55</definedName>
     <definedName name="_ftn1" localSheetId="0">'Data Dictionary'!$B$16</definedName>
     <definedName name="_ftnref1" localSheetId="0">'Data Dictionary'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913" calcMode="manual"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="335">
   <si>
     <t>Functional Area</t>
   </si>
@@ -262,9 +254,6 @@
     <t>q-applicant-have-you-applied-for-or-received-any-other-compensation</t>
   </si>
   <si>
-    <t>Yes/Yes, but I am still waiting for a decision/No</t>
-  </si>
-  <si>
     <t>q-applicant-who-did-you-apply-to</t>
   </si>
   <si>
@@ -280,9 +269,6 @@
     <t>p-applicant-enter-your-name</t>
   </si>
   <si>
-    <t>q-applicant-who-did-you-apply-to-still-waiting</t>
-  </si>
-  <si>
     <t>q-applicant-title</t>
   </si>
   <si>
@@ -355,9 +341,6 @@
     <t>Start now</t>
   </si>
   <si>
-    <t>residency_02</t>
-  </si>
-  <si>
     <t>is_injured_person</t>
   </si>
   <si>
@@ -416,9 +399,6 @@
   </si>
   <si>
     <t>APP_TITLE</t>
-  </si>
-  <si>
-    <t>other_claimant_name_01</t>
   </si>
   <si>
     <t>other_names</t>
@@ -867,11 +847,6 @@
     <t>Existing OAS question ID</t>
   </si>
   <si>
-    <t xml:space="preserve">• 'Start now' button must appear above 'Before you start'
-• Must have feedback loop built onto the page
-</t>
-  </si>
-  <si>
     <t>Functional requirements</t>
   </si>
   <si>
@@ -886,11 +861,6 @@
     <t xml:space="preserve">• Must write question and response to summary form
 • Must be shown on page if answer to q-applicant-have-you-applied-for-or-received-any-other-compensation is 'Yes'
 • Monetary value
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Must write question and response to summary form
-• Must be shown on page if answer to q-applicant-have-you-applied-for-or-received-any-other-compensation is 'Yes, but I am still waiting for a decision'
 </t>
   </si>
   <si>
@@ -951,15 +921,6 @@
 • Requires Google analytics to capture drop out rate from service from this page
 • Must include functionality for the user to go back to previous page
 • Must have feedback loop built onto the page</t>
-  </si>
-  <si>
-    <t>• Must write question and response to summary form if 'Yes'
-• Must present an error message if user attempts to continue without answering the question
-• Requires Google analytics to capture drop out rate from service from this page
-• Requires Google analytics to capture re-direct figures to old OAS
-• Must include functionality for the user to go back to previous page
-• Must have feedback loop built onto the page
-• Continue button must appear directly below text</t>
   </si>
   <si>
     <t>• Must write question and response to summary form if 'Myself'
@@ -994,17 +955,6 @@
 • Continue button must appear directly below text</t>
   </si>
   <si>
-    <t>• Must write question and response to summary form if 'Option 1'
-• Must present an error message if user attempts to continue without answering the question
-• Requires Google analytics to capture drop out rate from service from this page
-• Requires Google analytics to capture re-direct figures to old OAS
-• Must include functionality for the user to go back to previous page
-• Must have feedback loop built onto the page
-• Needs to include functionality to display information about DMI if user needs it
-• Needs to include functionality to display 'If you need help' guidance
-• Continue button must appear directly below text</t>
-  </si>
-  <si>
     <t>• Must write question and response to summary form
 • Must present an error message if user attempts to continue without answering the question
 • Requires Google analytics to capture drop out rate from service from this page
@@ -1028,27 +978,6 @@
 • Requires Google analytics to capture drop out rate from service from this page
 • Must include functionality for the user to go back to previous page
 • Must have feedback loop built onto the page
-• If answer is greater than 48 hours from date of submission,it must generate a 'Review Ineligible Application' task and allocated to TM8A for assessment
-• Continue button must appear directly below text</t>
-  </si>
-  <si>
-    <t>• Must write question and response to summary form
-• Must present an error message if user attempts to continue without answering the question
-• Requires Google analytics to capture drop out rate from service from this page
-• Must include functionality for the user to go back to previous page
-• Must have feedback loop built onto the page
-• Continue button must appear directly below text</t>
-  </si>
-  <si>
-    <t>• Must write question and response to summary form
-• Must present an error message if user attempts to continue without answering the question
-• Requires Google analytics to capture drop out rate from service from this page
-• Must include functionality for the user to go back to previous page
-• Must have feedback loop built onto the page
-• Must write back to TEMPUS as PI if 'Once' selected
-• Must write back to TEMPUS as POA if 'Period of time' selected
-• If 'Once' is selected, must be recorded for reporting purposes on Mangement Information tool as PI
-• If 'Period of time' selected, must be recorded for reporting purposes on Mangement Information tool as POA
 • Continue button must appear directly below text</t>
   </si>
   <si>
@@ -1064,63 +993,12 @@
   </si>
   <si>
     <t>• Must write question and response to summary form
-• Must be recorded for reporting purposes on Mangement Information tool
-• Must present an error message if user attempts to continue without answering the question
-• Requires Google analytics to capture drop out rate from service from this page
-• Must include functionality for the user to go back to previous page
-• Must have feedback loop built onto the page
-• Must have functionality to advise applicant how to find date if they do not know
-• Continue button must appear directly below text</t>
-  </si>
-  <si>
-    <t>• Must write question and response to summary form
-• Must present an error message if user attempts to continue without answering the question
-• Requires Google analytics to capture drop out rate from service from this page
-• Must include functionality for the user to go back to previous page
-• Must have feedback loop built onto the page
-• Must have functionality to advise applicant how to find date if they do not know
-• If delay betweem date of application and date of crime stop is 2 years or more, 'Review Ineligible Application' task must be genertated and allocated to TM1C for assessment
-• Continue button must appear directly below text</t>
-  </si>
-  <si>
-    <t>• Must write question and check box response to summary form
-• Must write 500 words from text box back to summary form
-• User must be able to check more than one reason
-• Must present an error message if user attempts to continue without answering the question
-• Requires Google analytics to capture drop out rate from service from this page
-• Must include functionality for the user to go back to previous page
-• Must have feedback loop built onto the page
-• Must have functionality to advise applicant how to find date if they do not know
-• Continue button must appear directly below text</t>
-  </si>
-  <si>
-    <t>• Must write question and response to summary form
 • Must present an error message if user attempts to continue without answering the question
 • Requires Google analytics to capture drop out rate from service from this page
 • Must include functionality for the user to go back to previous page
 • Must have feedback loop built onto the page
 • Must include content to advise applicant we will not contact offender
 • Continue button must appear directly below text</t>
-  </si>
-  <si>
-    <t>• Must write question and 500 words from text box back to summary form, or;
-• Must write question and check box response back to summary form
-• Must present an error message if user attempts to continue without answering the question
-• Requires Google analytics to capture drop out rate from service from this page
-• Must include functionality for the user to go back to previous page
-• Must have feedback loop built onto the page
-• If 'I have no contact with offender' is not selected and text is entered into free text box, 'Review Ineligible Application' task must be genertated and allocated to TM8A for assessment
-• Continue button must appear directly below text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">• Must write question and response to summary form
-• Must present an error message if user attempts to continue without answering the question
-• Requires Google analytics to capture drop out rate from service from this page
-• Must include functionality for the user to go back to previous page
-• Must have feedback loop built onto the page
-• If answer is 'Yes', once application is submitted it must generate a 'Review Ineligible Application' task and allocated to TM8A for assessment
-• Continue button must appear directly below text
-</t>
   </si>
   <si>
     <t>• Must write question and response to summary form
@@ -1208,13 +1086,6 @@
     <t>Optional</t>
   </si>
   <si>
-    <t>• Must write question and response to summary form
-• Must include ability to go back to previous page
-• Must have feedback loop built onto the page
-• Requires Google analytics to capture drop out rate from service from this page
-• Continue button must appear directly below text</t>
-  </si>
-  <si>
     <t>p-applicant-where-in-england-did-it-happen</t>
   </si>
   <si>
@@ -1267,15 +1138,6 @@
   </si>
   <si>
     <t>Drop down list</t>
-  </si>
-  <si>
-    <t>• Must write question and response to summary form 
-• Must be recorded for reporting purposes on Mangement Information tool
-• Must present an error message if user attempts to continue without answering the question
-• Requires Google analytics to capture drop out rate from service from this page
-• Must include functionality for the user to go back to previous page
-• Must have feedback loop built onto the page
-• Continue button must appear directly below list</t>
   </si>
   <si>
     <t xml:space="preserve">p--which-police-scotland-division-is-investigating-the-crime </t>
@@ -1540,12 +1402,195 @@
   <si>
     <t>English police forces</t>
   </si>
+  <si>
+    <t>• 'Start now' button must appear above 'Before you start'
+• Must have feedback loop built onto the page
+• Must include links to external sites: Northern Ireland/Victims and witness service/Relevant Place guidance</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Must write question and response to summary form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+• Must include ability to go back to previous page
+• Must have feedback loop built onto the page
+• Requires Google analytics to capture drop out rate from service from this page
+• Continue button must appear directly below text</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>• Must write question and response to summary form if 'Yes'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Requires Google analytics to capture re-direct figures to old OAS
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• Continue button must appear directly below text</t>
+    </r>
+  </si>
+  <si>
+    <t>• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Requires Google analytics to capture re-direct figures to old OAS
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• Continue button must appear directly below text</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Must write question and response to summary form if 'Option 1'
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Requires Google analytics to capture re-direct figures to old OAS
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• Needs to include functionality to display information about DMI if user needs it
+• Needs to include functionality to display 'If you need help' guidance
+• Continue button must appear directly below text
+• If Option 1 is selected, TEMPUS must allocate case to TM1C
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>• Must write to MI tool as...</t>
+    </r>
+  </si>
+  <si>
+    <t>• Must write question and response to summary form
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• If answer is greater than 2 days from date of incident,it must generate a 'Review Ineligible Application' task and allocated to TM8A for assessment
+• Continue button must appear directly below text</t>
+  </si>
+  <si>
+    <t>• Must write question and response to summary form
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• TEMPUS must identify if there is an end date and register the claim as 'POA' 
+• Once TEMPUS has identified if case is PI/POA, it must write back to MI tool
+• Continue button must appear directly below text</t>
+  </si>
+  <si>
+    <t>• Must write question and response to summary form
+• Must be recorded for reporting purposes on Mangement Information tool
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• Must have functionality to advise applicant how to find date if they do not know
+• Continue button must appear directly below text
+•  When mapping to TEMPUS, day must default to 01</t>
+  </si>
+  <si>
+    <t>• Must write question and response to summary form
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• Must have functionality to advise applicant how to find date if they do not know
+• If delay betweem date of application and date of crime stop is 2 years or more, 'Review Ineligible Application' task must be genertated and allocated to TM1C for assessment
+• Continue button must appear directly below text
+• When mapping to TEMPUS, day must default to 01</t>
+  </si>
+  <si>
+    <t>• Must write question and check box/free text response to summary form
+• Must write 500 characters from text box back to summary form
+• User must be able to check more than one reason
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• Must have functionality to advise applicant how to find date if they do not know
+• Continue button must appear directly below text</t>
+  </si>
+  <si>
+    <t>• Must write question and response to summary form 
+• Must be recorded for reporting purposes on Mangement Information tool
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• Continue button must appear directly below list
+• TEMPUS must use this question to allocate to correct regional case work area
+•  Must generate the police email based on ID</t>
+  </si>
+  <si>
+    <t>• Must write question and check box response to summary form (must concatenate responses)
+• Must write 500 characters from text box back to summary form
+• User must be able to check more than one reason
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• Must have functionality to advise applicant how to find date if they do not know
+• Continue button must appear directly below text</t>
+  </si>
+  <si>
+    <t>• Must write question and 500 characters from text box back to summary form, or;
+• Must write question and check box response back to summary form
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• If 'I have no contact with offender' is not selected and text is entered into free text box, 'Review Ineligible Application' task must be genertated and allocated to TM8A for assessment
+• Continue button must appear directly below text</t>
+  </si>
+  <si>
+    <t>• Must write question and response to summary form
+• Must present an error message if user attempts to continue without answering the question
+• Requires Google analytics to capture drop out rate from service from this page
+• Must include functionality for the user to go back to previous page
+• Must have feedback loop built onto the page
+• If answer is 'Yes', once application is submitted it must generate a 'Review Ineligible Application' task and allocated to TM8A for assessment
+• Continue button must appear directly below text</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="20" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1665,8 +1710,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1694,6 +1746,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1844,7 +1902,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1891,6 +1949,21 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1909,18 +1982,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2304,12 +2365,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L342"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L341"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2330,30 +2391,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="20"/>
+      <c r="A1" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="25"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>0</v>
@@ -2377,24 +2438,24 @@
         <v>2</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>17</v>
@@ -2403,7 +2464,7 @@
         <v>19</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H3" s="14" t="s">
         <v>12</v>
@@ -2415,13 +2476,13 @@
         <v>19</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>199</v>
+        <v>321</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="79.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>14</v>
       </c>
@@ -2429,7 +2490,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>13</v>
@@ -2444,7 +2505,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>19</v>
@@ -2453,13 +2514,13 @@
         <v>19</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>241</v>
+        <v>322</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
@@ -2467,10 +2528,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>3</v>
@@ -2491,10 +2552,10 @@
         <v>19</v>
       </c>
       <c r="K5" s="15" t="s">
-        <v>213</v>
+        <v>323</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="111" customHeight="1" x14ac:dyDescent="0.25">
@@ -2505,10 +2566,10 @@
         <v>22</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>3</v>
@@ -2529,10 +2590,10 @@
         <v>19</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>213</v>
+        <v>324</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="162" customHeight="1" x14ac:dyDescent="0.25">
@@ -2543,10 +2604,10 @@
         <v>24</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>3</v>
@@ -2567,10 +2628,10 @@
         <v>19</v>
       </c>
       <c r="K7" s="15" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -2581,10 +2642,10 @@
         <v>26</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>3</v>
@@ -2605,10 +2666,10 @@
         <v>19</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -2619,10 +2680,10 @@
         <v>19</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>17</v>
@@ -2643,10 +2704,10 @@
         <v>19</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -2657,10 +2718,10 @@
         <v>19</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>17</v>
@@ -2681,13 +2742,13 @@
         <v>19</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="178.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>29</v>
       </c>
@@ -2695,10 +2756,10 @@
         <v>30</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>3</v>
@@ -2719,13 +2780,13 @@
         <v>19</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>218</v>
+        <v>325</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="146.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>32</v>
       </c>
@@ -2733,10 +2794,10 @@
         <v>33</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>3</v>
@@ -2757,13 +2818,13 @@
         <v>19</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="L12" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="97.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>34</v>
       </c>
@@ -2771,10 +2832,10 @@
         <v>19</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>17</v>
@@ -2795,13 +2856,13 @@
         <v>19</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>35</v>
       </c>
@@ -2809,10 +2870,10 @@
         <v>36</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>37</v>
@@ -2833,13 +2894,13 @@
         <v>19</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>221</v>
+        <v>326</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>39</v>
       </c>
@@ -2847,10 +2908,10 @@
         <v>40</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>41</v>
@@ -2871,13 +2932,13 @@
         <v>30</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>42</v>
       </c>
@@ -2885,10 +2946,10 @@
         <v>43</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>3</v>
@@ -2900,7 +2961,7 @@
         <v>44</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>19</v>
@@ -2909,13 +2970,13 @@
         <v>19</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>223</v>
+        <v>327</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="150" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>45</v>
       </c>
@@ -2923,10 +2984,10 @@
         <v>46</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>37</v>
@@ -2947,13 +3008,13 @@
         <v>19</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="145.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>47</v>
       </c>
@@ -2961,10 +3022,10 @@
         <v>48</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>37</v>
@@ -2985,13 +3046,13 @@
         <v>19</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>225</v>
+        <v>328</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>50</v>
       </c>
@@ -2999,10 +3060,10 @@
         <v>51</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E19" s="14" t="s">
         <v>37</v>
@@ -3023,13 +3084,13 @@
         <v>19</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>226</v>
+        <v>329</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="144.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>55</v>
       </c>
@@ -3037,10 +3098,10 @@
         <v>56</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E20" s="14" t="s">
         <v>57</v>
@@ -3061,10 +3122,10 @@
         <v>500</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>227</v>
+        <v>330</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="105" x14ac:dyDescent="0.25">
@@ -3075,10 +3136,10 @@
         <v>53</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>3</v>
@@ -3099,24 +3160,24 @@
         <v>19</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>3</v>
@@ -3131,28 +3192,28 @@
         <v>11</v>
       </c>
       <c r="I22" s="14">
+        <v>60</v>
+      </c>
+      <c r="J22" s="14">
         <v>1</v>
       </c>
-      <c r="J22" s="14">
-        <v>60</v>
-      </c>
-      <c r="K22" s="27" t="s">
-        <v>232</v>
+      <c r="K22" s="18" t="s">
+        <v>217</v>
       </c>
       <c r="L22" s="16"/>
     </row>
-    <row r="23" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E23" s="14" t="s">
         <v>3</v>
@@ -3172,23 +3233,23 @@
       <c r="J23" s="14">
         <v>60</v>
       </c>
-      <c r="K23" s="27" t="s">
-        <v>222</v>
+      <c r="K23" s="18" t="s">
+        <v>213</v>
       </c>
       <c r="L23" s="16"/>
     </row>
     <row r="24" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>3</v>
@@ -3208,23 +3269,23 @@
       <c r="J24" s="14">
         <v>60</v>
       </c>
-      <c r="K24" s="27" t="s">
-        <v>232</v>
+      <c r="K24" s="18" t="s">
+        <v>217</v>
       </c>
       <c r="L24" s="16"/>
     </row>
     <row r="25" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E25" s="14" t="s">
         <v>3</v>
@@ -3244,23 +3305,23 @@
       <c r="J25" s="14">
         <v>60</v>
       </c>
-      <c r="K25" s="27" t="s">
-        <v>222</v>
+      <c r="K25" s="18" t="s">
+        <v>213</v>
       </c>
       <c r="L25" s="16"/>
     </row>
     <row r="26" spans="1:12" ht="113.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E26" s="14" t="s">
         <v>3</v>
@@ -3280,23 +3341,23 @@
       <c r="J26" s="14">
         <v>60</v>
       </c>
-      <c r="K26" s="27" t="s">
-        <v>232</v>
+      <c r="K26" s="18" t="s">
+        <v>217</v>
       </c>
       <c r="L26" s="16"/>
     </row>
     <row r="27" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E27" s="14" t="s">
         <v>3</v>
@@ -3316,32 +3377,32 @@
       <c r="J27" s="14">
         <v>60</v>
       </c>
-      <c r="K27" s="27" t="s">
+      <c r="K27" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="L27" s="16"/>
+    </row>
+    <row r="28" spans="1:12" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="L27" s="16"/>
-    </row>
-    <row r="28" spans="1:12" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>237</v>
-      </c>
       <c r="E28" s="14" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>4</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>337</v>
+        <v>320</v>
       </c>
       <c r="H28" s="14" t="s">
         <v>11</v>
@@ -3353,24 +3414,24 @@
         <v>19</v>
       </c>
       <c r="K28" s="15" t="s">
-        <v>260</v>
+        <v>331</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="184.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>261</v>
+        <v>244</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>262</v>
+        <v>245</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E29" s="14" t="s">
         <v>3</v>
@@ -3379,7 +3440,7 @@
         <v>4</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>263</v>
+        <v>246</v>
       </c>
       <c r="H29" s="14" t="s">
         <v>11</v>
@@ -3391,22 +3452,22 @@
         <v>19</v>
       </c>
       <c r="K29" s="15" t="s">
-        <v>260</v>
+        <v>331</v>
       </c>
       <c r="L29" s="16"/>
     </row>
-    <row r="30" spans="1:12" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="E30" s="14" t="s">
         <v>3</v>
@@ -3415,7 +3476,7 @@
         <v>4</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>265</v>
+        <v>248</v>
       </c>
       <c r="H30" s="14" t="s">
         <v>11</v>
@@ -3427,11 +3488,11 @@
         <v>19</v>
       </c>
       <c r="K30" s="15" t="s">
-        <v>260</v>
+        <v>331</v>
       </c>
       <c r="L30" s="16"/>
     </row>
-    <row r="31" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="144.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>59</v>
       </c>
@@ -3439,10 +3500,10 @@
         <v>60</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E31" s="14" t="s">
         <v>57</v>
@@ -3463,13 +3524,13 @@
         <v>500</v>
       </c>
       <c r="K31" s="15" t="s">
-        <v>227</v>
+        <v>332</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>62</v>
       </c>
@@ -3477,10 +3538,10 @@
         <v>63</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E32" s="14" t="s">
         <v>3</v>
@@ -3501,13 +3562,13 @@
         <v>19</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="L32" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>64</v>
       </c>
@@ -3515,10 +3576,10 @@
         <v>65</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E33" s="14" t="s">
         <v>3</v>
@@ -3539,10 +3600,10 @@
         <v>120</v>
       </c>
       <c r="K33" s="15" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="143.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3553,16 +3614,16 @@
         <v>68</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>3</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="G34" s="14" t="s">
         <v>66</v>
@@ -3576,11 +3637,11 @@
       <c r="J34" s="14">
         <v>500</v>
       </c>
-      <c r="K34" s="25" t="s">
-        <v>229</v>
+      <c r="K34" s="21" t="s">
+        <v>333</v>
       </c>
       <c r="L34" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -3588,22 +3649,22 @@
         <v>67</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="H35" s="14" t="s">
         <v>11</v>
@@ -3614,10 +3675,10 @@
       <c r="J35" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="K35" s="26"/>
+      <c r="K35" s="22"/>
       <c r="L35" s="16"/>
     </row>
-    <row r="36" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>69</v>
       </c>
@@ -3625,7 +3686,7 @@
         <v>70</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>71</v>
@@ -3649,10 +3710,10 @@
         <v>19</v>
       </c>
       <c r="K36" s="15" t="s">
-        <v>230</v>
+        <v>334</v>
       </c>
       <c r="L36" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -3663,7 +3724,7 @@
         <v>72</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D37" s="14" t="s">
         <v>71</v>
@@ -3672,7 +3733,7 @@
         <v>3</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="G37" s="14" t="s">
         <v>66</v>
@@ -3687,13 +3748,13 @@
         <v>15</v>
       </c>
       <c r="K37" s="15" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="L37" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="98.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>73</v>
       </c>
@@ -3701,7 +3762,7 @@
         <v>74</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>71</v>
@@ -3713,7 +3774,7 @@
         <v>4</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>75</v>
+        <v>8</v>
       </c>
       <c r="H38" s="14" t="s">
         <v>11</v>
@@ -3725,10 +3786,10 @@
         <v>19</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="L38" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3736,10 +3797,10 @@
         <v>73</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>71</v>
@@ -3763,10 +3824,10 @@
         <v>50</v>
       </c>
       <c r="K39" s="15" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="L39" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3774,19 +3835,19 @@
         <v>73</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D40" s="14" t="s">
         <v>71</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="G40" s="14" t="s">
         <v>66</v>
@@ -3801,10 +3862,10 @@
         <v>19</v>
       </c>
       <c r="K40" s="15" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L40" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3812,10 +3873,10 @@
         <v>73</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>71</v>
@@ -3836,27 +3897,27 @@
         <v>1</v>
       </c>
       <c r="J41" s="14">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
-        <v>73</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>123</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>71</v>
+        <v>220</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>3</v>
@@ -3864,7 +3925,7 @@
       <c r="F42" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="20" t="s">
         <v>66</v>
       </c>
       <c r="H42" s="14" t="s">
@@ -3874,27 +3935,27 @@
         <v>1</v>
       </c>
       <c r="J42" s="14">
-        <v>500</v>
+        <v>6</v>
       </c>
       <c r="K42" s="15" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="L42" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="118.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="D43" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E43" s="14" t="s">
         <v>3</v>
@@ -3912,27 +3973,27 @@
         <v>1</v>
       </c>
       <c r="J43" s="14">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="K43" s="15" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="L43" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="120" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>3</v>
@@ -3953,24 +4014,24 @@
         <v>70</v>
       </c>
       <c r="K44" s="15" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="L44" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="101.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>84</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E45" s="14" t="s">
         <v>3</v>
@@ -3979,25 +4040,25 @@
         <v>4</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="H45" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I45" s="14">
-        <v>1</v>
-      </c>
-      <c r="J45" s="14">
-        <v>70</v>
+      <c r="I45" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J45" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="K45" s="15" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="L45" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="102.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>85</v>
       </c>
@@ -4005,10 +4066,10 @@
         <v>86</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D46" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>3</v>
@@ -4017,25 +4078,25 @@
         <v>4</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="H46" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J46" s="14" t="s">
-        <v>19</v>
+      <c r="I46" s="14">
+        <v>1</v>
+      </c>
+      <c r="J46" s="14">
+        <v>50</v>
       </c>
       <c r="K46" s="15" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="L46" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="131.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>87</v>
       </c>
@@ -4043,86 +4104,86 @@
         <v>88</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>4</v>
       </c>
       <c r="G47" s="14" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="H47" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I47" s="14">
-        <v>1</v>
-      </c>
-      <c r="J47" s="14">
-        <v>50</v>
+      <c r="I47" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="K47" s="15" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="L47" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="F48" s="14" t="s">
         <v>4</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="H48" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I48" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J48" s="14" t="s">
-        <v>19</v>
+      <c r="I48" s="14">
+        <v>1</v>
+      </c>
+      <c r="J48" s="14">
+        <v>50</v>
       </c>
       <c r="K48" s="15" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="L48" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="101.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="14" t="s">
-        <v>93</v>
-      </c>
       <c r="C49" s="14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>3</v>
@@ -4140,27 +4201,27 @@
         <v>1</v>
       </c>
       <c r="J49" s="14">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="L49" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D50" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>3</v>
@@ -4181,24 +4242,24 @@
         <v>60</v>
       </c>
       <c r="K50" s="15" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="L50" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>3</v>
@@ -4219,30 +4280,30 @@
         <v>60</v>
       </c>
       <c r="K51" s="15" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="L51" s="16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>3</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="G52" s="14" t="s">
         <v>66</v>
@@ -4257,30 +4318,30 @@
         <v>60</v>
       </c>
       <c r="K52" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="L52" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="119.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E53" s="14" t="s">
         <v>3</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="G53" s="14" t="s">
         <v>66</v>
@@ -4292,33 +4353,33 @@
         <v>1</v>
       </c>
       <c r="J53" s="14">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="K53" s="15" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="L53" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>98</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E54" s="14" t="s">
         <v>3</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>240</v>
+        <v>4</v>
       </c>
       <c r="G54" s="14" t="s">
         <v>66</v>
@@ -4330,27 +4391,25 @@
         <v>1</v>
       </c>
       <c r="J54" s="14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
       <c r="L54" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="345.6" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B55" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14" t="s">
         <v>100</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>235</v>
       </c>
       <c r="E55" s="14" t="s">
         <v>3</v>
@@ -4359,59 +4418,37 @@
         <v>4</v>
       </c>
       <c r="G55" s="14" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="H55" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="I55" s="14">
-        <v>1</v>
-      </c>
-      <c r="J55" s="14">
-        <v>20</v>
+      <c r="I55" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="K55" s="15" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="L55" s="16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="345.6" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F56" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="H56" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="I56" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J56" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="K56" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="L56" s="16" t="s">
-        <v>195</v>
-      </c>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="8"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
@@ -4974,18 +5011,18 @@
       <c r="L96" s="8"/>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A97" s="8"/>
-      <c r="B97" s="9"/>
-      <c r="C97" s="9"/>
-      <c r="D97" s="9"/>
-      <c r="E97" s="9"/>
-      <c r="F97" s="9"/>
-      <c r="G97" s="9"/>
-      <c r="H97" s="9"/>
-      <c r="I97" s="9"/>
-      <c r="J97" s="9"/>
+      <c r="A97" s="7"/>
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+      <c r="E97" s="4"/>
+      <c r="F97" s="4"/>
+      <c r="G97" s="4"/>
+      <c r="H97" s="4"/>
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
       <c r="K97" s="6"/>
-      <c r="L97" s="8"/>
+      <c r="L97" s="7"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="7"/>
@@ -8403,31 +8440,17 @@
       <c r="K341" s="6"/>
       <c r="L341" s="7"/>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A342" s="7"/>
-      <c r="B342" s="4"/>
-      <c r="C342" s="4"/>
-      <c r="D342" s="4"/>
-      <c r="E342" s="4"/>
-      <c r="F342" s="4"/>
-      <c r="G342" s="4"/>
-      <c r="H342" s="4"/>
-      <c r="I342" s="5"/>
-      <c r="J342" s="5"/>
-      <c r="K342" s="6"/>
-      <c r="L342" s="7"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:L56"/>
+  <autoFilter ref="A2:L55" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="2">
     <mergeCell ref="K34:K35"/>
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L3" location="'Google Analytics'!A1" display="'Google Analytics'!A1"/>
-    <hyperlink ref="L4:L56" location="'Google Analytics'!A1" display="'Google Analytics'!A1"/>
-    <hyperlink ref="G28" location="'English police forces'!A1" display="English police forces"/>
+    <hyperlink ref="L3" location="'Google Analytics'!A1" display="'Google Analytics'!A1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="L4:L55" location="'Google Analytics'!A1" display="'Google Analytics'!A1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G28" location="'English police forces'!A1" display="English police forces" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="5" scale="84" orientation="landscape" r:id="rId1"/>
@@ -8436,11 +8459,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8452,392 +8475,392 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="10" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="A1" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
     </row>
     <row r="2" spans="1:4" s="12" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>146</v>
-      </c>
-      <c r="C4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5" t="s">
         <v>148</v>
-      </c>
-      <c r="B5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>151</v>
-      </c>
-      <c r="D5" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" t="s">
         <v>153</v>
-      </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D7" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" t="s">
         <v>162</v>
-      </c>
-      <c r="B11" t="s">
-        <v>146</v>
-      </c>
-      <c r="C11" t="s">
-        <v>165</v>
-      </c>
-      <c r="D11" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C16" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C17" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C18" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" t="s">
         <v>179</v>
-      </c>
-      <c r="B20" t="s">
-        <v>180</v>
-      </c>
-      <c r="C20" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" t="s">
         <v>180</v>
-      </c>
-      <c r="C21" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C22" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B23" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C23" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B24" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C24" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C25" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C26" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B27" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C27" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B28" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C28" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B29" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C29" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="22" t="s">
-        <v>194</v>
+      <c r="C32" s="27" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="23"/>
+      <c r="C33" s="28"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="23"/>
+      <c r="C34" s="28"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="23"/>
+      <c r="C35" s="28"/>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="23"/>
+      <c r="C36" s="28"/>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="23"/>
+      <c r="C37" s="28"/>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" s="23"/>
+      <c r="C38" s="28"/>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39" s="23"/>
+      <c r="C39" s="28"/>
     </row>
     <row r="40" spans="3:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="24"/>
+      <c r="C40" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8845,16 +8868,16 @@
     <mergeCell ref="C32:C40"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A29" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Individual URL, Event, Event - Reveal, Event - External, Filters, Report, Future possibilities"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B42" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Dev, Team"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A30:A32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A30:A32" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Individual URL, Event, Filters, Report, Future possibilities"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A33:A42">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A33:A42" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Individual URL, Event, Filters, Goal URL, Report"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8863,7 +8886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:B71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8874,353 +8897,353 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B11" s="19" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B15" s="19" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B16" s="19" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B18" s="19" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B19" s="19" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
+    <row r="20" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+    <row r="21" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B21" s="19" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+    <row r="22" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B22" s="19" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+    <row r="23" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B7" s="28" t="s">
+    <row r="24" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B24" s="19" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+    <row r="25" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B25" s="19" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
+    <row r="26" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B26" s="19" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+    <row r="27" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B27" s="19" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+    <row r="28" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B28" s="19" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B12" s="28" t="s">
+    <row r="29" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B29" s="19" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="13" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
+    <row r="30" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B30" s="19" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="14" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+    <row r="31" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B31" s="19" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
+    <row r="32" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B32" s="19" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="16" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
+    <row r="33" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B33" s="19" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
+    <row r="34" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B34" s="19" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
+    <row r="35" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B35" s="19" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="19" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
+    <row r="36" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B36" s="19" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+    <row r="37" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B37" s="19" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
+    <row r="38" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B38" s="19" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+    <row r="39" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B39" s="19" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
+    <row r="40" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B40" s="19" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B24" s="28" t="s">
+    <row r="41" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B41" s="19" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="25" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
+    <row r="42" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B42" s="19" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="26" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B26" s="28" t="s">
+    <row r="43" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B43" s="19" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="s">
+    <row r="44" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B44" s="19" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B28" s="28" t="s">
+    <row r="45" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B45" s="19" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B29" s="28" t="s">
+    <row r="46" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B46" s="19" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="30" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="s">
+    <row r="47" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B47" s="19" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B31" s="28" t="s">
+    <row r="48" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B48" s="19" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="32" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
+    <row r="49" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B49" s="19" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B33" s="28" t="s">
+    <row r="50" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B50" s="19" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B34" s="28" t="s">
+    <row r="51" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B51" s="19" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="35" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B35" s="28" t="s">
+    <row r="52" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B52" s="19" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="36" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B36" s="28" t="s">
+    <row r="53" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B53" s="19" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B37" s="28" t="s">
+    <row r="54" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B54" s="19" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="38" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B38" s="28" t="s">
+    <row r="55" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B55" s="19" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="39" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B39" s="28" t="s">
+    <row r="56" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B56" s="19" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="40" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B40" s="28" t="s">
+    <row r="57" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B57" s="19" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="41" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B41" s="28" t="s">
+    <row r="58" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B58" s="19" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="42" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B42" s="28" t="s">
+    <row r="59" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B59" s="19" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="43" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B43" s="28" t="s">
+    <row r="60" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B60" s="19" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B44" s="28" t="s">
+    <row r="61" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B61" s="19" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="45" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B45" s="28" t="s">
+    <row r="62" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B62" s="19" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="46" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B46" s="28" t="s">
+    <row r="63" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B63" s="19" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="47" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B47" s="28" t="s">
+    <row r="64" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B64" s="19" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="48" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B48" s="28" t="s">
+    <row r="65" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B65" s="19" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="49" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B49" s="28" t="s">
+    <row r="66" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B66" s="19" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="50" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B50" s="28" t="s">
+    <row r="67" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B67" s="19" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="51" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B51" s="28" t="s">
+    <row r="68" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B68" s="19" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="52" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B52" s="28" t="s">
+    <row r="69" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B69" s="19" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B53" s="28" t="s">
+    <row r="70" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B70" s="19" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B54" s="28" t="s">
+    <row r="71" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B71" s="19" t="s">
         <v>319</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B55" s="28" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B56" s="28" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B57" s="28" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B58" s="28" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B59" s="28" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B60" s="28" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B61" s="28" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B62" s="28" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B63" s="28" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B64" s="28" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B65" s="28" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B66" s="28" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B67" s="28" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B68" s="28" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B69" s="28" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B70" s="28" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B71" s="28" t="s">
-        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
review of data dictionary and feature files
</commit_message>
<xml_diff>
--- a/Data Dictionary.xlsx
+++ b/Data Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\q-definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB74AE2-6F0F-461A-AE69-7A074827E41D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4509EA62-4276-41F9-8EE0-3C453D406F88}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32772" yWindow="32772" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="345">
   <si>
     <t>Functional Area</t>
   </si>
@@ -1605,6 +1605,12 @@
   <si>
     <t>• This is the consent page for Private Beta, there are no requirements to write to summary
 • Must have hyperlink existing application</t>
+  </si>
+  <si>
+    <t>p--confirmation</t>
+  </si>
+  <si>
+    <t>• Reference number must be actual CICA reference</t>
   </si>
 </sst>
 </file>
@@ -1952,9 +1958,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1985,13 +1990,13 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2003,6 +2008,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2391,7 +2399,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2412,20 +2420,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="25"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="24"/>
     </row>
     <row r="2" spans="1:12" s="3" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2466,2187 +2474,2207 @@
       </c>
     </row>
     <row r="3" spans="1:12" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>340</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="L3" s="16"/>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" spans="1:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="79.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="111" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="L7" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="162" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="14" t="s">
         <v>200</v>
       </c>
-      <c r="L8" s="16" t="s">
+      <c r="L8" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="107.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="L9" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="61.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="K10" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="L10" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="14" t="s">
+      <c r="J11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="L11" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="178.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="J12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="L12" s="16" t="s">
+      <c r="L12" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="146.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="29" t="s">
         <v>325</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="J13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="15" t="s">
+      <c r="K13" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="L13" s="16" t="s">
+      <c r="L13" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="97.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="I14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="J14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="14" t="s">
         <v>205</v>
       </c>
-      <c r="L14" s="16" t="s">
+      <c r="L14" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="J15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K15" s="15" t="s">
+      <c r="K15" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="L15" s="16" t="s">
+      <c r="L15" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="14" t="s">
+      <c r="H16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="13">
         <v>1</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <v>30</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L16" s="16" t="s">
+      <c r="L16" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="14" t="s">
+      <c r="H17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="14" t="s">
+      <c r="I17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="L17" s="16" t="s">
+      <c r="L17" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H18" s="14" t="s">
+      <c r="H18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="J18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="L18" s="16" t="s">
+      <c r="L18" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="145.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="I19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="J19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="K19" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="L19" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="157.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="H20" s="14" t="s">
+      <c r="H20" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="14" t="s">
+      <c r="I20" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="J20" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="14" t="s">
         <v>321</v>
       </c>
-      <c r="L20" s="16" t="s">
+      <c r="L20" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="144.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="14" t="s">
+      <c r="H21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="14" t="s">
+      <c r="J21" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="15" t="s">
+      <c r="K21" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="144.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>333</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="14">
+      <c r="I22" s="13">
         <v>1</v>
       </c>
-      <c r="J22" s="14">
+      <c r="J22" s="13">
         <v>500</v>
       </c>
-      <c r="K22" s="15" t="s">
+      <c r="K22" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="L22" s="16"/>
+      <c r="L22" s="15"/>
     </row>
     <row r="23" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="14" t="s">
+      <c r="J23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="L23" s="16" t="s">
+      <c r="L23" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="29" t="s">
         <v>220</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="14">
+      <c r="I24" s="13">
         <v>1</v>
       </c>
-      <c r="J24" s="14">
+      <c r="J24" s="13">
         <v>60</v>
       </c>
-      <c r="K24" s="18" t="s">
+      <c r="K24" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="L24" s="16"/>
+      <c r="L24" s="15"/>
     </row>
     <row r="25" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H25" s="14" t="s">
+      <c r="H25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="14">
+      <c r="I25" s="13">
         <v>1</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25" s="13">
         <v>60</v>
       </c>
-      <c r="K25" s="18" t="s">
+      <c r="K25" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="L25" s="16"/>
+      <c r="L25" s="15"/>
     </row>
     <row r="26" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="H26" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I26" s="14">
+      <c r="I26" s="13">
         <v>1</v>
       </c>
-      <c r="J26" s="14">
+      <c r="J26" s="13">
         <v>60</v>
       </c>
-      <c r="K26" s="18" t="s">
+      <c r="K26" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="L26" s="16"/>
+      <c r="L26" s="15"/>
     </row>
     <row r="27" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="14" t="s">
+      <c r="G27" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H27" s="14" t="s">
+      <c r="H27" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I27" s="14">
+      <c r="I27" s="13">
         <v>1</v>
       </c>
-      <c r="J27" s="14">
+      <c r="J27" s="13">
         <v>60</v>
       </c>
-      <c r="K27" s="18" t="s">
+      <c r="K27" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="L27" s="16"/>
+      <c r="L27" s="15"/>
     </row>
     <row r="28" spans="1:12" ht="113.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="14" t="s">
+      <c r="F28" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="14" t="s">
+      <c r="H28" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="14">
+      <c r="I28" s="13">
         <v>1</v>
       </c>
-      <c r="J28" s="14">
+      <c r="J28" s="13">
         <v>60</v>
       </c>
-      <c r="K28" s="18" t="s">
+      <c r="K28" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="L28" s="16"/>
+      <c r="L28" s="15"/>
     </row>
     <row r="29" spans="1:12" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E29" s="14" t="s">
+      <c r="E29" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="14" t="s">
+      <c r="G29" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H29" s="14" t="s">
+      <c r="H29" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="14">
+      <c r="I29" s="13">
         <v>1</v>
       </c>
-      <c r="J29" s="14">
+      <c r="J29" s="13">
         <v>60</v>
       </c>
-      <c r="K29" s="18" t="s">
+      <c r="K29" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="L29" s="16"/>
+      <c r="L29" s="15"/>
     </row>
     <row r="30" spans="1:12" ht="139.80000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="29" t="s">
         <v>234</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="J30" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="15" t="s">
+      <c r="K30" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="L30" s="16" t="s">
+      <c r="L30" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="184.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="29" t="s">
         <v>237</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="H31" s="14" t="s">
+      <c r="H31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="I31" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="J31" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K31" s="15" t="s">
+      <c r="K31" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="L31" s="16"/>
+      <c r="L31" s="15"/>
     </row>
     <row r="32" spans="1:12" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="29" t="s">
         <v>334</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="E32" s="14" t="s">
+      <c r="E32" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G32" s="14" t="s">
+      <c r="G32" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="H32" s="14" t="s">
+      <c r="H32" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="J32" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K32" s="15" t="s">
+      <c r="K32" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="L32" s="16"/>
+      <c r="L32" s="15"/>
     </row>
     <row r="33" spans="1:12" ht="144.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G33" s="14" t="s">
+      <c r="G33" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="H33" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I33" s="14" t="s">
+      <c r="I33" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="14" t="s">
+      <c r="J33" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="15" t="s">
+      <c r="K33" s="14" t="s">
         <v>338</v>
       </c>
-      <c r="L33" s="16" t="s">
+      <c r="L33" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="144.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="29" t="s">
         <v>337</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H34" s="14" t="s">
+      <c r="H34" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I34" s="14">
+      <c r="I34" s="13">
         <v>1</v>
       </c>
-      <c r="J34" s="14">
+      <c r="J34" s="13">
         <v>500</v>
       </c>
-      <c r="K34" s="15" t="s">
+      <c r="K34" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="L34" s="16"/>
+      <c r="L34" s="15"/>
     </row>
     <row r="35" spans="1:12" ht="96.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F35" s="14" t="s">
+      <c r="F35" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G35" s="14" t="s">
+      <c r="G35" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H35" s="14" t="s">
+      <c r="H35" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I35" s="14" t="s">
+      <c r="I35" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="J35" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K35" s="15" t="s">
+      <c r="K35" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L35" s="16" t="s">
+      <c r="L35" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F36" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G36" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H36" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I36" s="14">
+      <c r="I36" s="13">
         <v>1</v>
       </c>
-      <c r="J36" s="14">
+      <c r="J36" s="13">
         <v>120</v>
       </c>
-      <c r="K36" s="15" t="s">
+      <c r="K36" s="14" t="s">
         <v>208</v>
       </c>
-      <c r="L36" s="16" t="s">
+      <c r="L36" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="143.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="D37" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="E37" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="G37" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="H37" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I37" s="14">
+      <c r="I37" s="13">
         <v>1</v>
       </c>
-      <c r="J37" s="14">
+      <c r="J37" s="13">
         <v>500</v>
       </c>
-      <c r="K37" s="21" t="s">
+      <c r="K37" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="L37" s="16" t="s">
+      <c r="L37" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="29" t="s">
         <v>331</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="C38" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D38" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="G38" s="14" t="s">
+      <c r="G38" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="H38" s="14" t="s">
+      <c r="H38" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I38" s="14" t="s">
+      <c r="I38" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J38" s="14" t="s">
+      <c r="J38" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K38" s="22"/>
-      <c r="L38" s="16"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="15"/>
     </row>
     <row r="39" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C39" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="D39" s="14" t="s">
+      <c r="D39" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="14" t="s">
+      <c r="G39" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H39" s="14" t="s">
+      <c r="H39" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I39" s="14" t="s">
+      <c r="I39" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J39" s="14" t="s">
+      <c r="J39" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K39" s="15" t="s">
+      <c r="K39" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="L39" s="16" t="s">
+      <c r="L39" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H40" s="14" t="s">
+      <c r="H40" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I40" s="14">
+      <c r="I40" s="13">
         <v>0</v>
       </c>
-      <c r="J40" s="14">
-        <v>15</v>
-      </c>
-      <c r="K40" s="15" t="s">
+      <c r="J40" s="13">
+        <v>50</v>
+      </c>
+      <c r="K40" s="14" t="s">
         <v>191</v>
       </c>
-      <c r="L40" s="16" t="s">
+      <c r="L40" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="98.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="14" t="s">
+      <c r="G41" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H41" s="14" t="s">
+      <c r="H41" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I41" s="14" t="s">
+      <c r="I41" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J41" s="14" t="s">
+      <c r="J41" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K41" s="15" t="s">
+      <c r="K41" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L41" s="16" t="s">
+      <c r="L41" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E42" s="14" t="s">
+      <c r="E42" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H42" s="14" t="s">
+      <c r="H42" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I42" s="14">
+      <c r="I42" s="13">
         <v>1</v>
       </c>
-      <c r="J42" s="14">
+      <c r="J42" s="13">
         <v>500</v>
       </c>
-      <c r="K42" s="15" t="s">
+      <c r="K42" s="14" t="s">
         <v>192</v>
       </c>
-      <c r="L42" s="16" t="s">
+      <c r="L42" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="14" t="s">
+      <c r="F43" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G43" s="14" t="s">
+      <c r="G43" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H43" s="14" t="s">
+      <c r="H43" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I43" s="14">
+      <c r="I43" s="13">
         <v>1</v>
       </c>
-      <c r="J43" s="14">
+      <c r="J43" s="13">
         <v>50</v>
       </c>
-      <c r="K43" s="15" t="s">
+      <c r="K43" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="L43" s="16" t="s">
+      <c r="L43" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C44" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D44" s="14" t="s">
+      <c r="D44" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E44" s="14" t="s">
+      <c r="E44" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="14" t="s">
+      <c r="G44" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H44" s="14" t="s">
+      <c r="H44" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I44" s="14" t="s">
+      <c r="I44" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J44" s="14" t="s">
+      <c r="J44" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K44" s="15" t="s">
+      <c r="K44" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="L44" s="16"/>
+      <c r="L44" s="15"/>
     </row>
     <row r="45" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="29" t="s">
         <v>329</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G45" s="14" t="s">
+      <c r="G45" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H45" s="14" t="s">
+      <c r="H45" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="14">
+      <c r="I45" s="13">
         <v>1</v>
       </c>
-      <c r="J45" s="14">
+      <c r="J45" s="13">
         <v>50</v>
       </c>
-      <c r="K45" s="15" t="s">
+      <c r="K45" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="L45" s="16"/>
+      <c r="L45" s="15"/>
     </row>
     <row r="46" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="16" t="s">
         <v>326</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="29" t="s">
         <v>330</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D46" s="14" t="s">
+      <c r="D46" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E46" s="14" t="s">
+      <c r="E46" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G46" s="14" t="s">
+      <c r="G46" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H46" s="14" t="s">
+      <c r="H46" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="14">
+      <c r="I46" s="13">
         <v>1</v>
       </c>
-      <c r="J46" s="14">
+      <c r="J46" s="13">
         <v>50</v>
       </c>
-      <c r="K46" s="15" t="s">
+      <c r="K46" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="L46" s="16"/>
+      <c r="L46" s="15"/>
     </row>
     <row r="47" spans="1:12" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C47" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="D47" s="14" t="s">
+      <c r="D47" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="F47" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G47" s="20" t="s">
+      <c r="G47" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="H47" s="14" t="s">
+      <c r="H47" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I47" s="14">
+      <c r="I47" s="13">
         <v>1</v>
       </c>
-      <c r="J47" s="14">
+      <c r="J47" s="13">
         <v>6</v>
       </c>
-      <c r="K47" s="15" t="s">
+      <c r="K47" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="L47" s="16" t="s">
+      <c r="L47" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="118.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="D48" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="E48" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F48" s="14" t="s">
+      <c r="F48" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G48" s="14" t="s">
+      <c r="G48" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H48" s="14" t="s">
+      <c r="H48" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I48" s="14">
+      <c r="I48" s="13">
         <v>1</v>
       </c>
-      <c r="J48" s="14">
+      <c r="J48" s="13">
         <v>70</v>
       </c>
-      <c r="K48" s="15" t="s">
+      <c r="K48" s="14" t="s">
         <v>195</v>
       </c>
-      <c r="L48" s="16" t="s">
+      <c r="L48" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D49" s="14" t="s">
+      <c r="D49" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E49" s="14" t="s">
+      <c r="E49" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F49" s="14" t="s">
+      <c r="F49" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="G49" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H49" s="14" t="s">
+      <c r="H49" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I49" s="14">
+      <c r="I49" s="13">
         <v>1</v>
       </c>
-      <c r="J49" s="14">
+      <c r="J49" s="13">
         <v>70</v>
       </c>
-      <c r="K49" s="15" t="s">
+      <c r="K49" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="L49" s="16" t="s">
+      <c r="L49" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="101.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F50" s="14" t="s">
+      <c r="F50" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G50" s="14" t="s">
+      <c r="G50" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H50" s="14" t="s">
+      <c r="H50" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I50" s="14" t="s">
+      <c r="I50" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J50" s="14" t="s">
+      <c r="J50" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K50" s="15" t="s">
+      <c r="K50" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L50" s="16" t="s">
+      <c r="L50" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="102.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C51" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="D51" s="14" t="s">
+      <c r="D51" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="E51" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F51" s="14" t="s">
+      <c r="F51" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G51" s="14" t="s">
+      <c r="G51" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H51" s="14" t="s">
+      <c r="H51" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I51" s="14">
+      <c r="I51" s="13">
         <v>1</v>
       </c>
-      <c r="J51" s="14">
+      <c r="J51" s="13">
         <v>50</v>
       </c>
-      <c r="K51" s="15" t="s">
+      <c r="K51" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="L51" s="16" t="s">
+      <c r="L51" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="131.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E52" s="14" t="s">
+      <c r="E52" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G52" s="14" t="s">
+      <c r="G52" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H52" s="14" t="s">
+      <c r="H52" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I52" s="14" t="s">
+      <c r="I52" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J52" s="14" t="s">
+      <c r="J52" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K52" s="15" t="s">
+      <c r="K52" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="L52" s="16" t="s">
+      <c r="L52" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="112.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F53" s="14" t="s">
+      <c r="F53" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G53" s="14" t="s">
+      <c r="G53" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H53" s="14" t="s">
+      <c r="H53" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I53" s="14">
+      <c r="I53" s="13">
         <v>1</v>
       </c>
-      <c r="J53" s="14">
+      <c r="J53" s="13">
         <v>50</v>
       </c>
-      <c r="K53" s="15" t="s">
+      <c r="K53" s="14" t="s">
         <v>211</v>
       </c>
-      <c r="L53" s="16" t="s">
+      <c r="L53" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="101.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D54" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="E54" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F54" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G54" s="14" t="s">
+      <c r="G54" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H54" s="14" t="s">
+      <c r="H54" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I54" s="14">
+      <c r="I54" s="13">
         <v>1</v>
       </c>
-      <c r="J54" s="14">
+      <c r="J54" s="13">
         <v>60</v>
       </c>
-      <c r="K54" s="15" t="s">
+      <c r="K54" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="L54" s="16" t="s">
+      <c r="L54" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E55" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F55" s="14" t="s">
+      <c r="F55" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G55" s="14" t="s">
+      <c r="G55" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H55" s="14" t="s">
+      <c r="H55" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I55" s="14">
+      <c r="I55" s="13">
         <v>1</v>
       </c>
-      <c r="J55" s="14">
+      <c r="J55" s="13">
         <v>60</v>
       </c>
-      <c r="K55" s="15" t="s">
+      <c r="K55" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="L55" s="16" t="s">
+      <c r="L55" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
+      <c r="A56" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D56" s="14" t="s">
+      <c r="D56" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E56" s="14" t="s">
+      <c r="E56" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F56" s="14" t="s">
+      <c r="F56" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G56" s="14" t="s">
+      <c r="G56" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H56" s="14" t="s">
+      <c r="H56" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I56" s="14">
+      <c r="I56" s="13">
         <v>1</v>
       </c>
-      <c r="J56" s="14">
+      <c r="J56" s="13">
         <v>60</v>
       </c>
-      <c r="K56" s="15" t="s">
+      <c r="K56" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="L56" s="16" t="s">
+      <c r="L56" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D57" s="14" t="s">
+      <c r="D57" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E57" s="14" t="s">
+      <c r="E57" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F57" s="14" t="s">
+      <c r="F57" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="G57" s="14" t="s">
+      <c r="G57" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H57" s="14" t="s">
+      <c r="H57" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I57" s="14">
+      <c r="I57" s="13">
         <v>1</v>
       </c>
-      <c r="J57" s="14">
+      <c r="J57" s="13">
         <v>60</v>
       </c>
-      <c r="K57" s="15" t="s">
+      <c r="K57" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="L57" s="16" t="s">
+      <c r="L57" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="119.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D58" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E58" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="G58" s="14" t="s">
+      <c r="G58" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H58" s="14" t="s">
+      <c r="H58" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I58" s="14">
+      <c r="I58" s="13">
         <v>1</v>
       </c>
-      <c r="J58" s="14">
+      <c r="J58" s="13">
         <v>10</v>
       </c>
-      <c r="K58" s="15" t="s">
+      <c r="K58" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="L58" s="16" t="s">
+      <c r="L58" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="90.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="D59" s="14" t="s">
+      <c r="D59" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="E59" s="14" t="s">
+      <c r="E59" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F59" s="14" t="s">
+      <c r="F59" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="14" t="s">
+      <c r="G59" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="H59" s="14" t="s">
+      <c r="H59" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I59" s="14">
+      <c r="I59" s="13">
         <v>1</v>
       </c>
-      <c r="J59" s="14">
+      <c r="J59" s="13">
         <v>20</v>
       </c>
-      <c r="K59" s="15" t="s">
+      <c r="K59" s="14" t="s">
         <v>194</v>
       </c>
-      <c r="L59" s="16" t="s">
+      <c r="L59" s="15" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="345.6" x14ac:dyDescent="0.25">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14" t="s">
+      <c r="C60" s="13"/>
+      <c r="D60" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="E60" s="14" t="s">
+      <c r="E60" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F60" s="14" t="s">
+      <c r="F60" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G60" s="14" t="s">
+      <c r="G60" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="H60" s="14" t="s">
+      <c r="H60" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I60" s="14" t="s">
+      <c r="I60" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J60" s="14" t="s">
+      <c r="J60" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K60" s="15" t="s">
+      <c r="K60" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="L60" s="16" t="s">
+      <c r="L60" s="15" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
-      <c r="J61" s="9"/>
-      <c r="K61" s="6"/>
+    <row r="61" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J61" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="K61" s="14" t="s">
+        <v>344</v>
+      </c>
       <c r="L61" s="8"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
@@ -8674,25 +8702,25 @@
     <col min="4" max="4" width="51.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="10" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-    </row>
-    <row r="2" spans="1:4" s="12" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+    </row>
+    <row r="2" spans="1:4" s="11" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>135</v>
       </c>
     </row>
@@ -8717,7 +8745,7 @@
       <c r="C4" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>141</v>
       </c>
     </row>
@@ -9034,33 +9062,33 @@
     </row>
     <row r="31" spans="1:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:3" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="26" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33" s="28"/>
+      <c r="C33" s="27"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C34" s="28"/>
+      <c r="C34" s="27"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="28"/>
+      <c r="C35" s="27"/>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C36" s="28"/>
+      <c r="C36" s="27"/>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C37" s="28"/>
+      <c r="C37" s="27"/>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C38" s="28"/>
+      <c r="C38" s="27"/>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C39" s="28"/>
+      <c r="C39" s="27"/>
     </row>
     <row r="40" spans="3:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="29"/>
+      <c r="C40" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9097,352 +9125,352 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="14" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="16" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="18" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="18" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="18" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="18" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="18" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="26" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="18" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="18" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="28" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="18" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="29" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="18" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="30" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="18" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="31" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="18" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="32" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="18" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B33" s="19" t="s">
+      <c r="B33" s="18" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B34" s="19" t="s">
+      <c r="B34" s="18" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="18" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="18" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="18" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B38" s="19" t="s">
+      <c r="B38" s="18" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="18" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="18" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="18" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="18" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="18" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="18" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="18" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="18" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="18" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B48" s="19" t="s">
+      <c r="B48" s="18" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B49" s="19" t="s">
+      <c r="B49" s="18" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B50" s="19" t="s">
+      <c r="B50" s="18" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="18" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="18" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="53" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="18" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="54" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B54" s="19" t="s">
+      <c r="B54" s="18" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="55" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B55" s="19" t="s">
+      <c r="B55" s="18" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="56" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B56" s="19" t="s">
+      <c r="B56" s="18" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="57" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B57" s="19" t="s">
+      <c r="B57" s="18" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="58" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B58" s="19" t="s">
+      <c r="B58" s="18" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="59" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="18" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="60" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B60" s="19" t="s">
+      <c r="B60" s="18" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="61" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B61" s="19" t="s">
+      <c r="B61" s="18" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="62" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B62" s="19" t="s">
+      <c r="B62" s="18" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="63" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="18" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="64" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B64" s="19" t="s">
+      <c r="B64" s="18" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="65" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B65" s="19" t="s">
+      <c r="B65" s="18" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="66" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="18" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="67" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B67" s="19" t="s">
+      <c r="B67" s="18" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="68" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="18" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="69" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B69" s="19" t="s">
+      <c r="B69" s="18" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="70" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B70" s="19" t="s">
+      <c r="B70" s="18" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="71" spans="2:2" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B71" s="19" t="s">
+      <c r="B71" s="18" t="s">
         <v>311</v>
       </c>
     </row>

</xml_diff>